<commit_message>
Do elimination properly. Test passes.
</commit_message>
<xml_diff>
--- a/tests/testthat/fixtures/metadata/metadata_no_timeval_or_codes.xlsx
+++ b/tests/testthat/fixtures/metadata/metadata_no_timeval_or_codes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\pxmake\tests\testthat\fixtures\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672C1394-686C-409A-B264-9003E7702DEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC556BF-2830-4A98-BEAF-9B2436438319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16680" yWindow="0" windowWidth="24210" windowHeight="31785" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="3900" windowWidth="43200" windowHeight="23445" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="59">
   <si>
     <t>keyword</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>d</t>
+  </si>
+  <si>
+    <t>en_elimination</t>
   </si>
 </sst>
 </file>
@@ -276,15 +279,16 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table5" displayName="Table5" ref="A1:F4" totalsRowShown="0">
-  <autoFilter ref="A1:F4" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table5" displayName="Table5" ref="A1:G4" totalsRowShown="0">
+  <autoFilter ref="A1:G4" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="pivot"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="order"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="variable-code"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="type"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="en_variable-label"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="en_note"/>
+    <tableColumn id="7" xr3:uid="{144F3902-8CA8-4D33-8101-D8540659A835}" name="en_elimination"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -835,10 +839,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,9 +853,10 @@
     <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -870,8 +875,11 @@
       <c r="F1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -885,7 +893,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -899,7 +907,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -1050,7 +1058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>

</xml_diff>